<commit_message>
More work on window2 class
</commit_message>
<xml_diff>
--- a/moscow/Chess game MoSCoW chart.xlsx
+++ b/moscow/Chess game MoSCoW chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff25509d146f77ad/Desktop/Chess-Game/.gitignore/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff25509d146f77ad/Desktop/Chess-Game/moscow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{E1D34FEC-D034-4771-AD00-E5FFB1B0FAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E7C977-936C-4B48-9808-75EEFCC160FE}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="8_{E1D34FEC-D034-4771-AD00-E5FFB1B0FAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EB4B799-C290-46B7-99F9-775D77C8B973}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{B81DFFB1-29F3-4B43-838E-C705C1ECE243}"/>
+    <workbookView xWindow="12390" yWindow="0" windowWidth="12660" windowHeight="16010" xr2:uid="{B81DFFB1-29F3-4B43-838E-C705C1ECE243}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Must</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Export current position to FEN</t>
+  </si>
+  <si>
+    <t>Be able to highlight squares/draw arrows</t>
   </si>
 </sst>
 </file>
@@ -203,12 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -233,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A0264FF-E12F-4604-A5B1-DB28CFDE1D73}" name="Table2" displayName="Table2" ref="A1:D17" totalsRowShown="0">
-  <autoFilter ref="A1:D17" xr:uid="{8A0264FF-E12F-4604-A5B1-DB28CFDE1D73}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A0264FF-E12F-4604-A5B1-DB28CFDE1D73}" name="Table2" displayName="Table2" ref="A1:D19" totalsRowShown="0">
+  <autoFilter ref="A1:D19" xr:uid="{8A0264FF-E12F-4604-A5B1-DB28CFDE1D73}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -547,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADAA543-B46A-408A-87D9-BCC70DD167FB}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,131 +581,130 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
@@ -711,18 +712,18 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -737,6 +738,11 @@
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>